<commit_message>
Envio del ultimo Producto
</commit_message>
<xml_diff>
--- a/Algoritmos/Prestamo_Ejemplo.xlsx
+++ b/Algoritmos/Prestamo_Ejemplo.xlsx
@@ -495,22 +495,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9891403742729185</v>
+        <v>0.9887804249359229</v>
       </c>
       <c r="E2" t="n">
         <v>25000</v>
       </c>
       <c r="F2" t="n">
-        <v>298.86</v>
+        <v>289.76</v>
       </c>
       <c r="G2" t="n">
-        <v>274.47</v>
+        <v>283.67</v>
       </c>
       <c r="H2" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -529,22 +529,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" t="n">
-        <v>0.978398680016769</v>
+        <v>0.978042639594854</v>
       </c>
       <c r="E3" t="n">
-        <v>24701.14</v>
+        <v>24710.24</v>
       </c>
       <c r="F3" t="n">
-        <v>302.15</v>
+        <v>302.14</v>
       </c>
       <c r="G3" t="n">
-        <v>271.19</v>
+        <v>271.29</v>
       </c>
       <c r="H3" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -563,22 +563,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" t="n">
-        <v>0.967421462583727</v>
+        <v>0.9670694167840513</v>
       </c>
       <c r="E4" t="n">
-        <v>24398.99</v>
+        <v>24408.11</v>
       </c>
       <c r="F4" t="n">
-        <v>296.48</v>
+        <v>296.47</v>
       </c>
       <c r="G4" t="n">
-        <v>276.85</v>
+        <v>276.96</v>
       </c>
       <c r="H4" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -597,22 +597,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9569156275797217</v>
+        <v>0.9565674048656693</v>
       </c>
       <c r="E5" t="n">
-        <v>24102.51</v>
+        <v>24111.63</v>
       </c>
       <c r="F5" t="n">
-        <v>308.72</v>
+        <v>308.71</v>
       </c>
       <c r="G5" t="n">
-        <v>264.62</v>
+        <v>264.72</v>
       </c>
       <c r="H5" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -631,22 +631,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9465238820118106</v>
+        <v>0.9461794408661025</v>
       </c>
       <c r="E6" t="n">
-        <v>23793.79</v>
+        <v>23802.92</v>
       </c>
       <c r="F6" t="n">
-        <v>312.11</v>
+        <v>312.1</v>
       </c>
       <c r="G6" t="n">
-        <v>261.23</v>
+        <v>261.33</v>
       </c>
       <c r="H6" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -665,22 +665,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9362449869114179</v>
+        <v>0.9359042862676371</v>
       </c>
       <c r="E7" t="n">
-        <v>23481.68</v>
+        <v>23490.82</v>
       </c>
       <c r="F7" t="n">
         <v>315.53</v>
       </c>
       <c r="G7" t="n">
-        <v>257.8</v>
+        <v>257.9</v>
       </c>
       <c r="H7" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -699,22 +699,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9257407160023993</v>
+        <v>0.9254038378750659</v>
       </c>
       <c r="E8" t="n">
-        <v>23166.15</v>
+        <v>23175.3</v>
       </c>
       <c r="F8" t="n">
-        <v>310.47</v>
+        <v>310.46</v>
       </c>
       <c r="G8" t="n">
-        <v>262.86</v>
+        <v>262.97</v>
       </c>
       <c r="H8" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -733,22 +733,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9156875183062926</v>
+        <v>0.9153542985493377</v>
       </c>
       <c r="E9" t="n">
-        <v>22855.68</v>
+        <v>22864.84</v>
       </c>
       <c r="F9" t="n">
-        <v>322.41</v>
+        <v>322.4</v>
       </c>
       <c r="G9" t="n">
-        <v>250.93</v>
+        <v>251.03</v>
       </c>
       <c r="H9" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -767,22 +767,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9054138934594166</v>
+        <v>0.9050844122865377</v>
       </c>
       <c r="E10" t="n">
-        <v>22533.27</v>
+        <v>22542.44</v>
       </c>
       <c r="F10" t="n">
-        <v>317.65</v>
+        <v>317.64</v>
       </c>
       <c r="G10" t="n">
-        <v>255.68</v>
+        <v>255.79</v>
       </c>
       <c r="H10" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -801,22 +801,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8952555343176902</v>
+        <v>0.8949297497835627</v>
       </c>
       <c r="E11" t="n">
-        <v>22215.62</v>
+        <v>22224.8</v>
       </c>
       <c r="F11" t="n">
-        <v>321.26</v>
+        <v>321.25</v>
       </c>
       <c r="G11" t="n">
-        <v>252.08</v>
+        <v>252.18</v>
       </c>
       <c r="H11" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -835,22 +835,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8855333942849016</v>
+        <v>0.8852111476488823</v>
       </c>
       <c r="E12" t="n">
-        <v>21894.36</v>
+        <v>21903.55</v>
       </c>
       <c r="F12" t="n">
-        <v>332.96</v>
+        <v>332.95</v>
       </c>
       <c r="G12" t="n">
-        <v>240.37</v>
+        <v>240.48</v>
       </c>
       <c r="H12" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -869,22 +869,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8752794547302778</v>
+        <v>0.8749609395148337</v>
       </c>
       <c r="E13" t="n">
-        <v>21561.4</v>
+        <v>21570.6</v>
       </c>
       <c r="F13" t="n">
-        <v>320.74</v>
+        <v>320.73</v>
       </c>
       <c r="G13" t="n">
-        <v>252.59</v>
+        <v>252.7</v>
       </c>
       <c r="H13" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -903,22 +903,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8660894183957957</v>
+        <v>0.8657742474453028</v>
       </c>
       <c r="E14" t="n">
-        <v>21240.66</v>
+        <v>21249.87</v>
       </c>
       <c r="F14" t="n">
         <v>347.95</v>
       </c>
       <c r="G14" t="n">
-        <v>225.38</v>
+        <v>225.48</v>
       </c>
       <c r="H14" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -937,22 +937,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8563722631539011</v>
+        <v>0.8560606282875454</v>
       </c>
       <c r="E15" t="n">
-        <v>20892.71</v>
+        <v>20901.92</v>
       </c>
       <c r="F15" t="n">
-        <v>336.27</v>
+        <v>336.26</v>
       </c>
       <c r="G15" t="n">
-        <v>237.07</v>
+        <v>237.17</v>
       </c>
       <c r="H15" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -971,22 +971,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8467641302646522</v>
+        <v>0.8464559918090723</v>
       </c>
       <c r="E16" t="n">
-        <v>20556.44</v>
+        <v>20565.67</v>
       </c>
       <c r="F16" t="n">
-        <v>340.08</v>
+        <v>340.07</v>
       </c>
       <c r="G16" t="n">
-        <v>233.25</v>
+        <v>233.36</v>
       </c>
       <c r="H16" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1005,22 +1005,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8381785060096403</v>
+        <v>0.8378734918727501</v>
       </c>
       <c r="E17" t="n">
-        <v>20216.36</v>
+        <v>20225.6</v>
       </c>
       <c r="F17" t="n">
-        <v>366.26</v>
+        <v>366.25</v>
       </c>
       <c r="G17" t="n">
-        <v>207.08</v>
+        <v>207.17</v>
       </c>
       <c r="H17" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1039,22 +1039,22 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D18" t="n">
-        <v>0.828774499344369</v>
+        <v>0.8284729073364833</v>
       </c>
       <c r="E18" t="n">
-        <v>19850.1</v>
+        <v>19859.34</v>
       </c>
       <c r="F18" t="n">
-        <v>348.1</v>
+        <v>348.09</v>
       </c>
       <c r="G18" t="n">
-        <v>225.24</v>
+        <v>225.34</v>
       </c>
       <c r="H18" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1073,22 +1073,22 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8197743184693398</v>
+        <v>0.8194760016377819</v>
       </c>
       <c r="E19" t="n">
-        <v>19502</v>
+        <v>19511.26</v>
       </c>
       <c r="F19" t="n">
-        <v>359.23</v>
+        <v>359.22</v>
       </c>
       <c r="G19" t="n">
-        <v>214.11</v>
+        <v>214.21</v>
       </c>
       <c r="H19" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1107,22 +1107,22 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8105767989676703</v>
+        <v>0.810281829124197</v>
       </c>
       <c r="E20" t="n">
-        <v>19142.78</v>
+        <v>19152.04</v>
       </c>
       <c r="F20" t="n">
-        <v>356.12</v>
+        <v>356.11</v>
       </c>
       <c r="G20" t="n">
-        <v>217.21</v>
+        <v>217.32</v>
       </c>
       <c r="H20" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1141,22 +1141,22 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8017742383078256</v>
+        <v>0.801482471726453</v>
       </c>
       <c r="E21" t="n">
-        <v>18786.65</v>
+        <v>18795.93</v>
       </c>
       <c r="F21" t="n">
-        <v>367.08</v>
+        <v>367.07</v>
       </c>
       <c r="G21" t="n">
-        <v>206.26</v>
+        <v>206.36</v>
       </c>
       <c r="H21" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -1175,22 +1175,22 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7924901789723761</v>
+        <v>0.7922017908710347</v>
       </c>
       <c r="E22" t="n">
-        <v>18419.57</v>
+        <v>18428.86</v>
       </c>
       <c r="F22" t="n">
-        <v>357.55</v>
+        <v>357.53</v>
       </c>
       <c r="G22" t="n">
-        <v>215.79</v>
+        <v>215.89</v>
       </c>
       <c r="H22" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1209,22 +1209,22 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7838840322363481</v>
+        <v>0.7835987759218515</v>
       </c>
       <c r="E23" t="n">
-        <v>18062.02</v>
+        <v>18071.32</v>
       </c>
       <c r="F23" t="n">
         <v>375.03</v>
       </c>
       <c r="G23" t="n">
-        <v>198.3</v>
+        <v>198.4</v>
       </c>
       <c r="H23" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1249,16 +1249,16 @@
         <v>0.7753713450328257</v>
       </c>
       <c r="E24" t="n">
-        <v>17686.99</v>
+        <v>17696.3</v>
       </c>
       <c r="F24" t="n">
-        <v>379.15</v>
+        <v>385.65</v>
       </c>
       <c r="G24" t="n">
-        <v>194.18</v>
+        <v>187.77</v>
       </c>
       <c r="H24" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1283,16 +1283,16 @@
         <v>0.7666720080246955</v>
       </c>
       <c r="E25" t="n">
-        <v>17307.84</v>
+        <v>17310.64</v>
       </c>
       <c r="F25" t="n">
-        <v>376.95</v>
+        <v>377.01</v>
       </c>
       <c r="G25" t="n">
-        <v>196.39</v>
+        <v>196.42</v>
       </c>
       <c r="H25" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -1317,16 +1317,16 @@
         <v>0.7583462369621171</v>
       </c>
       <c r="E26" t="n">
-        <v>16930.89</v>
+        <v>16933.64</v>
       </c>
       <c r="F26" t="n">
-        <v>387.45</v>
+        <v>387.52</v>
       </c>
       <c r="G26" t="n">
-        <v>185.88</v>
+        <v>185.91</v>
       </c>
       <c r="H26" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1351,16 +1351,16 @@
         <v>0.7498379144319601</v>
       </c>
       <c r="E27" t="n">
-        <v>16543.44</v>
+        <v>16546.12</v>
       </c>
       <c r="F27" t="n">
-        <v>385.62</v>
+        <v>385.68</v>
       </c>
       <c r="G27" t="n">
-        <v>187.72</v>
+        <v>187.75</v>
       </c>
       <c r="H27" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -1385,16 +1385,16 @@
         <v>0.7414250516650996</v>
       </c>
       <c r="E28" t="n">
-        <v>16157.82</v>
+        <v>16160.44</v>
       </c>
       <c r="F28" t="n">
-        <v>389.99</v>
+        <v>390.06</v>
       </c>
       <c r="G28" t="n">
-        <v>183.34</v>
+        <v>183.37</v>
       </c>
       <c r="H28" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -1419,16 +1419,16 @@
         <v>0.7339074955011891</v>
       </c>
       <c r="E29" t="n">
-        <v>15767.83</v>
+        <v>15770.38</v>
       </c>
       <c r="F29" t="n">
-        <v>411.82</v>
+        <v>411.89</v>
       </c>
       <c r="G29" t="n">
-        <v>161.51</v>
+        <v>161.54</v>
       </c>
       <c r="H29" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -1453,16 +1453,16 @@
         <v>0.7256733652653247</v>
       </c>
       <c r="E30" t="n">
-        <v>15356</v>
+        <v>15358.49</v>
       </c>
       <c r="F30" t="n">
-        <v>399.09</v>
+        <v>399.16</v>
       </c>
       <c r="G30" t="n">
-        <v>174.24</v>
+        <v>174.27</v>
       </c>
       <c r="H30" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -1487,16 +1487,16 @@
         <v>0.7175316184717289</v>
       </c>
       <c r="E31" t="n">
-        <v>14956.91</v>
+        <v>14959.34</v>
       </c>
       <c r="F31" t="n">
-        <v>403.62</v>
+        <v>403.69</v>
       </c>
       <c r="G31" t="n">
-        <v>169.71</v>
+        <v>169.74</v>
       </c>
       <c r="H31" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -1521,16 +1521,16 @@
         <v>0.7097394936477787</v>
       </c>
       <c r="E32" t="n">
-        <v>14553.29</v>
+        <v>14555.65</v>
       </c>
       <c r="F32" t="n">
-        <v>413.56</v>
+        <v>413.62</v>
       </c>
       <c r="G32" t="n">
-        <v>159.78</v>
+        <v>159.8</v>
       </c>
       <c r="H32" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -1555,16 +1555,16 @@
         <v>0.7020319883830354</v>
       </c>
       <c r="E33" t="n">
-        <v>14139.73</v>
+        <v>14142.03</v>
       </c>
       <c r="F33" t="n">
-        <v>418.1</v>
+        <v>418.16</v>
       </c>
       <c r="G33" t="n">
-        <v>155.24</v>
+        <v>155.26</v>
       </c>
       <c r="H33" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -1589,16 +1589,16 @@
         <v>0.6941554877919885</v>
       </c>
       <c r="E34" t="n">
-        <v>13721.64</v>
+        <v>13723.86</v>
       </c>
       <c r="F34" t="n">
-        <v>417.64</v>
+        <v>417.71</v>
       </c>
       <c r="G34" t="n">
-        <v>155.7</v>
+        <v>155.72</v>
       </c>
       <c r="H34" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -1623,16 +1623,16 @@
         <v>0.6863673581905653</v>
       </c>
       <c r="E35" t="n">
-        <v>13304</v>
+        <v>13306.16</v>
       </c>
       <c r="F35" t="n">
-        <v>422.38</v>
+        <v>422.44</v>
       </c>
       <c r="G35" t="n">
-        <v>150.96</v>
+        <v>150.98</v>
       </c>
       <c r="H35" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -1657,16 +1657,16 @@
         <v>0.6789136655693299</v>
       </c>
       <c r="E36" t="n">
-        <v>12881.62</v>
+        <v>12883.71</v>
       </c>
       <c r="F36" t="n">
-        <v>431.91</v>
+        <v>431.98</v>
       </c>
       <c r="G36" t="n">
-        <v>141.43</v>
+        <v>141.45</v>
       </c>
       <c r="H36" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -1691,16 +1691,16 @@
         <v>0.671296542736447</v>
       </c>
       <c r="E37" t="n">
-        <v>12449.71</v>
+        <v>12451.73</v>
       </c>
       <c r="F37" t="n">
-        <v>432.07</v>
+        <v>432.14</v>
       </c>
       <c r="G37" t="n">
-        <v>141.27</v>
+        <v>141.29</v>
       </c>
       <c r="H37" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -1725,16 +1725,16 @@
         <v>0.6640065135304454</v>
       </c>
       <c r="E38" t="n">
-        <v>12017.64</v>
+        <v>12019.59</v>
       </c>
       <c r="F38" t="n">
-        <v>441.4</v>
+        <v>441.47</v>
       </c>
       <c r="G38" t="n">
-        <v>131.94</v>
+        <v>131.96</v>
       </c>
       <c r="H38" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -1759,16 +1759,16 @@
         <v>0.6563177208800948</v>
       </c>
       <c r="E39" t="n">
-        <v>11576.25</v>
+        <v>11578.12</v>
       </c>
       <c r="F39" t="n">
-        <v>437.72</v>
+        <v>437.79</v>
       </c>
       <c r="G39" t="n">
-        <v>135.62</v>
+        <v>135.64</v>
       </c>
       <c r="H39" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -1793,16 +1793,16 @@
         <v>0.6491903560732858</v>
       </c>
       <c r="E40" t="n">
-        <v>11138.53</v>
+        <v>11140.33</v>
       </c>
       <c r="F40" t="n">
-        <v>451.05</v>
+        <v>451.12</v>
       </c>
       <c r="G40" t="n">
-        <v>122.29</v>
+        <v>122.31</v>
       </c>
       <c r="H40" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -1827,16 +1827,16 @@
         <v>0.6426079982855503</v>
       </c>
       <c r="E41" t="n">
-        <v>10687.48</v>
+        <v>10689.21</v>
       </c>
       <c r="F41" t="n">
-        <v>463.86</v>
+        <v>463.94</v>
       </c>
       <c r="G41" t="n">
-        <v>109.47</v>
+        <v>109.49</v>
       </c>
       <c r="H41" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -1861,16 +1861,16 @@
         <v>0.6353982096120091</v>
       </c>
       <c r="E42" t="n">
-        <v>10223.62</v>
+        <v>10225.28</v>
       </c>
       <c r="F42" t="n">
-        <v>457.33</v>
+        <v>457.4</v>
       </c>
       <c r="G42" t="n">
-        <v>116.01</v>
+        <v>116.03</v>
       </c>
       <c r="H42" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -1895,16 +1895,16 @@
         <v>0.6284980228679649</v>
       </c>
       <c r="E43" t="n">
-        <v>9766.290000000001</v>
+        <v>9767.870000000001</v>
       </c>
       <c r="F43" t="n">
-        <v>466.11</v>
+        <v>466.19</v>
       </c>
       <c r="G43" t="n">
-        <v>107.22</v>
+        <v>107.24</v>
       </c>
       <c r="H43" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -1929,16 +1929,16 @@
         <v>0.6214465421227736</v>
       </c>
       <c r="E44" t="n">
-        <v>9300.18</v>
+        <v>9301.690000000001</v>
       </c>
       <c r="F44" t="n">
-        <v>467.81</v>
+        <v>467.88</v>
       </c>
       <c r="G44" t="n">
-        <v>105.53</v>
+        <v>105.55</v>
       </c>
       <c r="H44" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -1963,16 +1963,16 @@
         <v>0.6146978652659312</v>
       </c>
       <c r="E45" t="n">
-        <v>8832.370000000001</v>
+        <v>8833.799999999999</v>
       </c>
       <c r="F45" t="n">
-        <v>476.37</v>
+        <v>476.44</v>
       </c>
       <c r="G45" t="n">
-        <v>96.97</v>
+        <v>96.98999999999999</v>
       </c>
       <c r="H45" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -1997,16 +1997,16 @@
         <v>0.6078012164248522</v>
       </c>
       <c r="E46" t="n">
-        <v>8356.01</v>
+        <v>8357.360000000001</v>
       </c>
       <c r="F46" t="n">
-        <v>478.52</v>
+        <v>478.6</v>
       </c>
       <c r="G46" t="n">
-        <v>94.81</v>
+        <v>94.83</v>
       </c>
       <c r="H46" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -2031,16 +2031,16 @@
         <v>0.6009819450531361</v>
       </c>
       <c r="E47" t="n">
-        <v>7877.48</v>
+        <v>7878.76</v>
       </c>
       <c r="F47" t="n">
-        <v>483.95</v>
+        <v>484.03</v>
       </c>
       <c r="G47" t="n">
-        <v>89.38</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="H47" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
@@ -2065,16 +2065,16 @@
         <v>0.5942391830084572</v>
       </c>
       <c r="E48" t="n">
-        <v>7393.53</v>
+        <v>7394.73</v>
       </c>
       <c r="F48" t="n">
-        <v>489.44</v>
+        <v>489.52</v>
       </c>
       <c r="G48" t="n">
-        <v>83.89</v>
+        <v>83.91</v>
       </c>
       <c r="H48" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -2099,16 +2099,16 @@
         <v>0.5877859678886187</v>
       </c>
       <c r="E49" t="n">
-        <v>6904.09</v>
+        <v>6905.21</v>
       </c>
       <c r="F49" t="n">
-        <v>497.54</v>
+        <v>497.62</v>
       </c>
       <c r="G49" t="n">
-        <v>75.8</v>
+        <v>75.81</v>
       </c>
       <c r="H49" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -2133,16 +2133,16 @@
         <v>0.5814028322697178</v>
       </c>
       <c r="E50" t="n">
-        <v>6406.56</v>
+        <v>6407.59</v>
       </c>
       <c r="F50" t="n">
-        <v>503</v>
+        <v>503.08</v>
       </c>
       <c r="G50" t="n">
-        <v>70.34</v>
+        <v>70.34999999999999</v>
       </c>
       <c r="H50" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -2167,16 +2167,16 @@
         <v>0.5748797395506007</v>
       </c>
       <c r="E51" t="n">
-        <v>5903.56</v>
+        <v>5904.51</v>
       </c>
       <c r="F51" t="n">
-        <v>506.35</v>
+        <v>506.43</v>
       </c>
       <c r="G51" t="n">
-        <v>66.98999999999999</v>
+        <v>67</v>
       </c>
       <c r="H51" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -2201,16 +2201,16 @@
         <v>0.5684298331598956</v>
       </c>
       <c r="E52" t="n">
-        <v>5397.21</v>
+        <v>5398.08</v>
       </c>
       <c r="F52" t="n">
-        <v>512.09</v>
+        <v>512.1799999999999</v>
       </c>
       <c r="G52" t="n">
-        <v>61.24</v>
+        <v>61.25</v>
       </c>
       <c r="H52" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -2235,16 +2235,16 @@
         <v>0.5624615783446917</v>
       </c>
       <c r="E53" t="n">
-        <v>4885.12</v>
+        <v>4885.91</v>
       </c>
       <c r="F53" t="n">
-        <v>521.5</v>
+        <v>521.58</v>
       </c>
       <c r="G53" t="n">
         <v>51.84</v>
       </c>
       <c r="H53" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
@@ -2269,16 +2269,16 @@
         <v>0.5561509984457941</v>
       </c>
       <c r="E54" t="n">
-        <v>4363.62</v>
+        <v>4364.32</v>
       </c>
       <c r="F54" t="n">
-        <v>523.8200000000001</v>
+        <v>523.91</v>
       </c>
       <c r="G54" t="n">
-        <v>49.51</v>
+        <v>49.52</v>
       </c>
       <c r="H54" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -2303,16 +2303,16 @@
         <v>0.55011140675493</v>
       </c>
       <c r="E55" t="n">
-        <v>3839.79</v>
+        <v>3840.42</v>
       </c>
       <c r="F55" t="n">
-        <v>531.1799999999999</v>
+        <v>531.26</v>
       </c>
       <c r="G55" t="n">
         <v>42.16</v>
       </c>
       <c r="H55" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
@@ -2337,16 +2337,16 @@
         <v>0.5439393905332379</v>
       </c>
       <c r="E56" t="n">
-        <v>3308.62</v>
+        <v>3309.15</v>
       </c>
       <c r="F56" t="n">
-        <v>535.79</v>
+        <v>535.88</v>
       </c>
       <c r="G56" t="n">
-        <v>37.54</v>
+        <v>37.55</v>
       </c>
       <c r="H56" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -2371,16 +2371,16 @@
         <v>0.5380324123338301</v>
       </c>
       <c r="E57" t="n">
-        <v>2772.82</v>
+        <v>2773.27</v>
       </c>
       <c r="F57" t="n">
-        <v>542.89</v>
+        <v>542.98</v>
       </c>
       <c r="G57" t="n">
-        <v>30.44</v>
+        <v>30.45</v>
       </c>
       <c r="H57" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
@@ -2405,16 +2405,16 @@
         <v>0.5319959172967441</v>
       </c>
       <c r="E58" t="n">
-        <v>2229.93</v>
+        <v>2230.29</v>
       </c>
       <c r="F58" t="n">
-        <v>548.03</v>
+        <v>548.12</v>
       </c>
       <c r="G58" t="n">
-        <v>25.3</v>
+        <v>25.31</v>
       </c>
       <c r="H58" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
@@ -2439,16 +2439,16 @@
         <v>0.525835727275144</v>
       </c>
       <c r="E59" t="n">
-        <v>1681.9</v>
+        <v>1682.17</v>
       </c>
       <c r="F59" t="n">
-        <v>553.63</v>
+        <v>553.72</v>
       </c>
       <c r="G59" t="n">
-        <v>19.7</v>
+        <v>19.71</v>
       </c>
       <c r="H59" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
@@ -2473,16 +2473,16 @@
         <v>0.5203146912065932</v>
       </c>
       <c r="E60" t="n">
-        <v>1128.27</v>
+        <v>1128.45</v>
       </c>
       <c r="F60" t="n">
-        <v>561.36</v>
+        <v>561.45</v>
       </c>
       <c r="G60" t="n">
         <v>11.97</v>
       </c>
       <c r="H60" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
@@ -2507,16 +2507,16 @@
         <v>0.5144769814716588</v>
       </c>
       <c r="E61" t="n">
-        <v>566.9</v>
+        <v>566.99</v>
       </c>
       <c r="F61" t="n">
-        <v>566.9</v>
+        <v>566.99</v>
       </c>
       <c r="G61" t="n">
         <v>6.43</v>
       </c>
       <c r="H61" t="n">
-        <v>573.34</v>
+        <v>573.4299999999999</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>

</xml_diff>